<commit_message>
Added climber motor and cleaned up SRX configurations
</commit_message>
<xml_diff>
--- a/Doc/Robot IO.xlsx
+++ b/Doc/Robot IO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t xml:space="preserve">Robot I/O</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">pivot arm 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">climber</t>
   </si>
 </sst>
 </file>
@@ -361,7 +364,7 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -784,7 +787,9 @@
       <c r="A14" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="C14" s="8"/>
       <c r="D14" s="9"/>
       <c r="E14" s="7" t="n">

</xml_diff>

<commit_message>
Changed solenoid names in excel doc
</commit_message>
<xml_diff>
--- a/Doc/Robot IO.xlsx
+++ b/Doc/Robot IO.xlsx
@@ -79,7 +79,7 @@
     <t xml:space="preserve">Limit Switch 2</t>
   </si>
   <si>
-    <t xml:space="preserve">left intake</t>
+    <t xml:space="preserve">extend intake</t>
   </si>
   <si>
     <t xml:space="preserve">right motor 1</t>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Beam Break</t>
   </si>
   <si>
-    <t xml:space="preserve">right intake</t>
+    <t xml:space="preserve">open intake</t>
   </si>
   <si>
     <t xml:space="preserve">right motor 2</t>
@@ -363,8 +363,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added camera pole motor.  Control not complete
</commit_message>
<xml_diff>
--- a/Doc/Robot IO.xlsx
+++ b/Doc/Robot IO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t xml:space="preserve">Robot I/O</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t xml:space="preserve">climber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">camera pole</t>
   </si>
 </sst>
 </file>
@@ -363,8 +366,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -816,7 +819,9 @@
       <c r="A15" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="C15" s="8"/>
       <c r="D15" s="9"/>
       <c r="E15" s="7"/>

</xml_diff>